<commit_message>
change the navigationto IFELSE
</commit_message>
<xml_diff>
--- a/src/test/resources/Levels/tested Levels.xlsx
+++ b/src/test/resources/Levels/tested Levels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Samira\Ph.D\OnlineSearch\src\test\resources\Levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{637F0724-F853-4315-93BB-6B2859551BA7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69E3E9E-CC4B-40E0-A922-2BD1F5DB541F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{32A06598-CE81-4A90-9E9F-88E734A0E334}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{32A06598-CE81-4A90-9E9F-88E734A0E334}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
   <si>
     <t>status</t>
   </si>
@@ -172,6 +172,12 @@
   <si>
     <t>too comlicated,
 the same reason</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>agent fraized</t>
   </si>
 </sst>
 </file>
@@ -528,10 +534,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218B7203-4BAC-4C88-83D3-576C8CD635DD}">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,7 +549,7 @@
     <col min="5" max="5" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -560,7 +566,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -574,7 +580,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -588,7 +594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -602,7 +608,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -616,7 +622,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -630,7 +636,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -638,7 +644,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -652,7 +658,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -666,7 +672,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -679,8 +685,11 @@
       <c r="D10" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G10" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -693,8 +702,11 @@
       <c r="D11" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="87" x14ac:dyDescent="0.35">
+      <c r="G11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="87" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -707,8 +719,11 @@
       <c r="E12" s="3" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -719,7 +734,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -732,8 +747,11 @@
       <c r="E14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -746,8 +764,11 @@
       <c r="D15" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -760,8 +781,11 @@
       <c r="D16" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -774,8 +798,11 @@
       <c r="E17" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -790,6 +817,9 @@
       </c>
       <c r="E18" t="s">
         <v>39</v>
+      </c>
+      <c r="G18" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
solve the problem of sharing memory
</commit_message>
<xml_diff>
--- a/src/test/resources/Levels/tested Levels.xlsx
+++ b/src/test/resources/Levels/tested Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Samira\Ph.D\OnlineSearch\src\test\resources\Levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69E3E9E-CC4B-40E0-A922-2BD1F5DB541F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204FE7A8-5D50-4C4E-9686-58303223816B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{32A06598-CE81-4A90-9E9F-88E734A0E334}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
   <si>
     <t>status</t>
   </si>
@@ -178,6 +178,28 @@
   </si>
   <si>
     <t>agent fraized</t>
+  </si>
+  <si>
+    <t>D&amp;D first level</t>
+  </si>
+  <si>
+    <t>4  mis</t>
+  </si>
+  <si>
+    <t>s 5/6</t>
+  </si>
+  <si>
+    <t>s  5/5 1mis
+3times tried</t>
+  </si>
+  <si>
+    <t>s 2/4</t>
+  </si>
+  <si>
+    <t>s 8/11</t>
+  </si>
+  <si>
+    <t>s  8/11</t>
   </si>
 </sst>
 </file>
@@ -534,10 +556,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218B7203-4BAC-4C88-83D3-576C8CD635DD}">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -549,7 +571,7 @@
     <col min="5" max="5" width="22.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -566,7 +588,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -580,7 +602,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -594,7 +616,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -608,7 +630,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -622,7 +644,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -636,7 +658,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -644,7 +666,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -658,7 +680,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -672,7 +694,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -688,8 +710,11 @@
       <c r="G10" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -705,8 +730,11 @@
       <c r="G11" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="87" x14ac:dyDescent="0.35">
+      <c r="J11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -722,8 +750,11 @@
       <c r="G12" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J12" s="3" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -734,7 +765,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -750,8 +781,11 @@
       <c r="G14" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J14" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -767,8 +801,11 @@
       <c r="G15" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -784,8 +821,11 @@
       <c r="G16" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J16" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -801,8 +841,11 @@
       <c r="G17" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="J17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -820,6 +863,20 @@
       </c>
       <c r="G18" t="s">
         <v>44</v>
+      </c>
+      <c r="J18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>46</v>
+      </c>
+      <c r="I20" t="s">
+        <v>44</v>
+      </c>
+      <c r="J20" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding a test file with data collectore and get the result
</commit_message>
<xml_diff>
--- a/src/test/resources/Levels/tested Levels.xlsx
+++ b/src/test/resources/Levels/tested Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Samira\Ph.D\OnlineSearch\src\test\resources\Levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{204FE7A8-5D50-4C4E-9686-58303223816B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A772A05D-C8CE-48A3-AA0B-F1C76613A657}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{32A06598-CE81-4A90-9E9F-88E734A0E334}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
   <si>
     <t>status</t>
   </si>
@@ -99,13 +99,7 @@
     <t>OR4_3_3_M -&gt; same as CR_3_3</t>
   </si>
   <si>
-    <t>door6</t>
-  </si>
-  <si>
     <t>BM2021_diff1_R4_1_1</t>
-  </si>
-  <si>
-    <t>door5</t>
   </si>
   <si>
     <t>BM2021_diff1_R4_1_1_M</t>
@@ -200,16 +194,65 @@
   </si>
   <si>
     <t>s  8/11</t>
+  </si>
+  <si>
+    <t>door3 / (18,0,4)</t>
+  </si>
+  <si>
+    <t>door5(28,0,4)</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">door6 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(38,0,7)</t>
+    </r>
+  </si>
+  <si>
+    <t>door4(40,0,6)</t>
+  </si>
+  <si>
+    <t>door6(34,0,8)</t>
+  </si>
+  <si>
+    <t>door6(37,0,7)</t>
+  </si>
+  <si>
+    <t>door3(7,0,15)</t>
+  </si>
+  <si>
+    <t>doorEntrance (43,00,14)</t>
+  </si>
+  <si>
+    <t>second level</t>
+  </si>
+  <si>
+    <t>doorKey4(67,0,77)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -556,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218B7203-4BAC-4C88-83D3-576C8CD635DD}">
-  <dimension ref="A1:J20"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -655,7 +698,7 @@
         <v>14</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -691,7 +734,7 @@
         <v>14</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.35">
@@ -702,184 +745,196 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>51</v>
       </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="G10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>21</v>
+        <v>53</v>
       </c>
       <c r="D11" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="87" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>52</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
-        <v>31</v>
-      </c>
       <c r="C14" t="s">
-        <v>2</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J14" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B15" t="s">
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="G15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J15" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="D16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="G16" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J16" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" t="s">
         <v>11</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>57</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J17" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B18" t="s">
         <v>11</v>
       </c>
       <c r="C18" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="G18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J18" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
       </c>
       <c r="I20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="J20" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add multirun and multitasks classes
</commit_message>
<xml_diff>
--- a/src/test/resources/Levels/tested Levels.xlsx
+++ b/src/test/resources/Levels/tested Levels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Samira\Ph.D\OnlineSearch\src\test\resources\Levels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/s_shirzadehhajimahmood_uu_nl/Documents/Samira/Ph.D/OnlineSearch/src/test/resources/Levels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF3CB586-CF80-4946-8FA6-A373DBE74F01}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260DC5B7-8E1B-4356-A8DF-48253BE2EE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{32A06598-CE81-4A90-9E9F-88E734A0E334}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{32A06598-CE81-4A90-9E9F-88E734A0E334}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="103">
   <si>
     <t>status</t>
   </si>
@@ -236,6 +236,164 @@
   </si>
   <si>
     <t>doorKey4(67,0,77)</t>
+  </si>
+  <si>
+    <t>original level</t>
+  </si>
+  <si>
+    <t>selected level</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>killed!</t>
+  </si>
+  <si>
+    <t>BM2021_diff1_R3_1_1_H</t>
+  </si>
+  <si>
+    <t>button1_door1_4_BM2021_diff1_R3_1_1_H</t>
+  </si>
+  <si>
+    <t>button1-&gt;6 ….door1</t>
+  </si>
+  <si>
+    <t>button2_door3_3_BM2021_diff1_R3_1_1_H</t>
+  </si>
+  <si>
+    <t>button2-&gt;5 ….door3</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>""</t>
+  </si>
+  <si>
+    <t>button3_door2_0_BM2021_diff1_R3_1_1_H</t>
+  </si>
+  <si>
+    <t>button3-&gt;1…...door2</t>
+  </si>
+  <si>
+    <t>button3_door2_1_BM2021_diff1_R3_1_1_H</t>
+  </si>
+  <si>
+    <t>the agent died but was solvable</t>
+  </si>
+  <si>
+    <t>button3-&gt;2 ….door2</t>
+  </si>
+  <si>
+    <t>button6_door4_0_BM2021_diff1_R3_1_1_H</t>
+  </si>
+  <si>
+    <t>button6-&gt;1 …...door4</t>
+  </si>
+  <si>
+    <t>sequence : b1d1b2dT// b3d2b2dT</t>
+  </si>
+  <si>
+    <t>BM2021_diff1_R3_1_1_H-removing-dT</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>BM2021_diff1_R3_1_1_H-removing-b2</t>
+  </si>
+  <si>
+    <t>button2_door2_0_BM2021_diff1_R4_1_1</t>
+  </si>
+  <si>
+    <t>button4_door4_0_BM2021_diff1_R4_1_1</t>
+  </si>
+  <si>
+    <t>button2-&gt;1….door2</t>
+  </si>
+  <si>
+    <t>button4-&gt;1….door4</t>
+  </si>
+  <si>
+    <t>button4_door4_2_BM2021_diff1_R4_1_1</t>
+  </si>
+  <si>
+    <t>button4-&gt;3…..door4</t>
+  </si>
+  <si>
+    <t>button6_door5_2_BM2021_diff1_R4_1_1</t>
+  </si>
+  <si>
+    <t>button6-&gt;3…....door5</t>
+  </si>
+  <si>
+    <t>door2_BM2021_diff1_R4_1_1</t>
+  </si>
+  <si>
+    <t>door2 removed</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <r>
+      <t>b1d1b5d3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>b6d5b8d6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>//b2d2d4d4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>b6d5b8d6</t>
+    </r>
+  </si>
+  <si>
+    <t>BM2021_diff1_R4_1_1-removing-d6</t>
+  </si>
+  <si>
+    <t>door6 removed</t>
+  </si>
+  <si>
+    <t>BM2021_diff1_R4_1_1-removing-d5</t>
+  </si>
+  <si>
+    <t>door5 removed</t>
+  </si>
+  <si>
+    <t>BM2021_diff1_R4_1_1-removingb8</t>
+  </si>
+  <si>
+    <t>button8 removed</t>
+  </si>
+  <si>
+    <t>BM2021_diff1_R4_1_1-removingb6</t>
+  </si>
+  <si>
+    <t>button6 removed</t>
   </si>
 </sst>
 </file>
@@ -258,18 +416,59 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -278,13 +477,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -599,19 +801,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218B7203-4BAC-4C88-83D3-576C8CD635DD}">
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J47"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="41.36328125" customWidth="1"/>
-    <col min="2" max="2" width="18.08984375" customWidth="1"/>
+    <col min="2" max="2" width="39.36328125" customWidth="1"/>
     <col min="3" max="3" width="49.7265625" customWidth="1"/>
     <col min="4" max="4" width="29.1796875" customWidth="1"/>
-    <col min="5" max="5" width="22.81640625" customWidth="1"/>
+    <col min="5" max="5" width="42.36328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -933,6 +1135,264 @@
         <v>60</v>
       </c>
     </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A26" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A27" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E27" s="4"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A28" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E28" s="4"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A29" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E29" s="4"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="E30" s="4"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E31" s="4"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A32" s="4"/>
+      <c r="B32" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E32" s="4"/>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A33" s="4"/>
+      <c r="B33" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="D33" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="E33" s="4"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A34" s="4"/>
+      <c r="B34" s="4"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A35" s="4"/>
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A36" s="4"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A37" s="4"/>
+      <c r="B37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A38" s="4"/>
+      <c r="B38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E39" s="4"/>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A40" s="4"/>
+      <c r="B40" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E40" s="4"/>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A41" s="4"/>
+      <c r="B41" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E41" s="4"/>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A42" s="4"/>
+      <c r="B42" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E42" s="4"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B43" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E43" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B44" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
+        <v>99</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D46" s="5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B47" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C47" t="s">
+        <v>102</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
final result and changes
</commit_message>
<xml_diff>
--- a/src/test/resources/Levels/tested Levels.xlsx
+++ b/src/test/resources/Levels/tested Levels.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://solisservices-my.sharepoint.com/personal/s_shirzadehhajimahmood_uu_nl/Documents/Samira/Ph.D/OnlineSearch/src/test/resources/Levels/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{260DC5B7-8E1B-4356-A8DF-48253BE2EE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{260DC5B7-8E1B-4356-A8DF-48253BE2EE21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED439B7E-2E21-4A91-BCD4-80E3BF0C7F05}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{32A06598-CE81-4A90-9E9F-88E734A0E334}"/>
   </bookViews>
@@ -803,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{218B7203-4BAC-4C88-83D3-576C8CD635DD}">
   <dimension ref="A1:J47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>